<commit_message>
Certificate name solved - Coursera - Matrix ongoing
</commit_message>
<xml_diff>
--- a/7_MATHS/2_Matrix/1_Matrices.xlsx
+++ b/7_MATHS/2_Matrix/1_Matrices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\7_MATHS\2_Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A4BF8D-3BD2-457D-A049-63A242738882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E937BF-81E6-440B-BE47-642EBB781664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Matrix A</t>
   </si>
@@ -66,6 +88,18 @@
   </si>
   <si>
     <t>BA</t>
+  </si>
+  <si>
+    <t>C . B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A . D</t>
+  </si>
+  <si>
+    <t>D. A</t>
   </si>
 </sst>
 </file>
@@ -107,12 +141,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -142,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +197,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K28"/>
+  <dimension ref="B2:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -764,7 +813,242 @@
         <v>16</v>
       </c>
     </row>
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="F31" s="3">
+        <v>4</v>
+      </c>
+      <c r="G31" s="3">
+        <v>-2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3">
+        <v>-4</v>
+      </c>
+      <c r="H32" s="3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" cm="1">
+        <f t="array" ref="B36:D37">MMULT(B31:C32,F31:H32)</f>
+        <v>8</v>
+      </c>
+      <c r="C36" s="8">
+        <v>-10</v>
+      </c>
+      <c r="D36" s="8">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37" s="8">
+        <v>10</v>
+      </c>
+      <c r="C37" s="8">
+        <v>-8</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>3</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3">
+        <v>3</v>
+      </c>
+      <c r="D42" s="3">
+        <v>4</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" cm="1">
+        <f t="array" ref="B45:D47">MMULT(B40:D42,F40:H42)</f>
+        <v>2</v>
+      </c>
+      <c r="C45" s="8">
+        <v>3</v>
+      </c>
+      <c r="D45" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
+        <v>2</v>
+      </c>
+      <c r="C46" s="8">
+        <v>6</v>
+      </c>
+      <c r="D46" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="8">
+        <v>2</v>
+      </c>
+      <c r="C47" s="8">
+        <v>9</v>
+      </c>
+      <c r="D47" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" cm="1">
+        <f t="array" ref="B50:D52">MMULT(F40:H42,B40:D42)</f>
+        <v>2</v>
+      </c>
+      <c r="C50" s="8">
+        <v>2</v>
+      </c>
+      <c r="D50" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" s="8">
+        <v>3</v>
+      </c>
+      <c r="C51" s="8">
+        <v>6</v>
+      </c>
+      <c r="D51" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52" s="8">
+        <v>4</v>
+      </c>
+      <c r="C52" s="8">
+        <v>12</v>
+      </c>
+      <c r="D52" s="8">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Matrix inverse and alike
</commit_message>
<xml_diff>
--- a/7_MATHS/2_Matrix/1_Matrices.xlsx
+++ b/7_MATHS/2_Matrix/1_Matrices.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\7_MATHS\2_Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E937BF-81E6-440B-BE47-642EBB781664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02E7D16-5FA0-490E-A7E8-CD22487116CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Matrix A</t>
   </si>
@@ -100,19 +101,168 @@
   </si>
   <si>
     <t>D. A</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>U. V</t>
+  </si>
+  <si>
+    <t>3 x 1</t>
+  </si>
+  <si>
+    <t>1 x 3</t>
+  </si>
+  <si>
+    <t>3 x 3</t>
+  </si>
+  <si>
+    <t>Outer Product</t>
+  </si>
+  <si>
+    <t>Inner Product</t>
+  </si>
+  <si>
+    <t>1 x 1</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A . </t>
+  </si>
+  <si>
+    <t>Sum of diagonal elements</t>
+  </si>
+  <si>
+    <t>B = A</t>
+  </si>
+  <si>
+    <t>Sum of square of all elements of A</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>A. B</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. B </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> . A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -140,8 +290,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +323,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,31 +372,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -865,39 +1085,31 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-    </row>
     <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" cm="1">
+      <c r="B36" s="7" cm="1">
         <f t="array" ref="B36:D37">MMULT(B31:C32,F31:H32)</f>
         <v>8</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>-10</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="7">
         <v>-3</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="8">
+      <c r="B37" s="7">
         <v>10</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>-8</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="7">
         <v>0</v>
       </c>
     </row>
@@ -970,81 +1182,541 @@
       </c>
     </row>
     <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" cm="1">
+      <c r="B45" s="7" cm="1">
         <f t="array" ref="B45:D47">MMULT(B40:D42,F40:H42)</f>
         <v>2</v>
       </c>
-      <c r="C45" s="8">
-        <v>3</v>
-      </c>
-      <c r="D45" s="8">
+      <c r="C45" s="7">
+        <v>3</v>
+      </c>
+      <c r="D45" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="8">
-        <v>2</v>
-      </c>
-      <c r="C46" s="8">
+      <c r="B46" s="7">
+        <v>2</v>
+      </c>
+      <c r="C46" s="7">
         <v>6</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="7">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="8">
-        <v>2</v>
-      </c>
-      <c r="C47" s="8">
+      <c r="B47" s="7">
+        <v>2</v>
+      </c>
+      <c r="C47" s="7">
         <v>9</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" cm="1">
+      <c r="B50" s="7" cm="1">
         <f t="array" ref="B50:D52">MMULT(F40:H42,B40:D42)</f>
         <v>2</v>
       </c>
-      <c r="C50" s="8">
-        <v>2</v>
-      </c>
-      <c r="D50" s="8">
+      <c r="C50" s="7">
+        <v>2</v>
+      </c>
+      <c r="D50" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="8">
-        <v>3</v>
-      </c>
-      <c r="C51" s="8">
+      <c r="B51" s="7">
+        <v>3</v>
+      </c>
+      <c r="C51" s="7">
         <v>6</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D51" s="7">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="8">
-        <v>4</v>
-      </c>
-      <c r="C52" s="8">
+      <c r="B52" s="7">
+        <v>4</v>
+      </c>
+      <c r="C52" s="7">
         <v>12</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="7">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EA0345-A843-4158-A3B6-4BAA3FA7F133}">
+  <dimension ref="B2:K51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="9.140625" style="10"/>
+    <col min="6" max="6" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" cm="1">
+        <f t="array" ref="B9:D11">MMULT(B4:B6,F4:H4)</f>
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>15</v>
+      </c>
+      <c r="D11" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9">
+        <v>3</v>
+      </c>
+      <c r="F15" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" cm="1">
+        <f t="array" ref="B20">MMULT(B15:D15,F15:F17)</f>
+        <v>32</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="2:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="2:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="2:11" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="J23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9">
+        <v>2</v>
+      </c>
+      <c r="H24" s="9">
+        <v>3</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="9">
+        <v>4</v>
+      </c>
+      <c r="G25" s="9">
+        <v>5</v>
+      </c>
+      <c r="H25" s="9">
+        <v>6</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2</v>
+      </c>
+      <c r="K25" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="J26" s="3">
+        <v>3</v>
+      </c>
+      <c r="K26" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="18" cm="1">
+        <f t="array" ref="B28:D30">MMULT(B24:C26,F24:H25)</f>
+        <v>17</v>
+      </c>
+      <c r="C28" s="18">
+        <v>22</v>
+      </c>
+      <c r="D28" s="18">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B29" s="18">
+        <v>22</v>
+      </c>
+      <c r="C29" s="18">
+        <v>29</v>
+      </c>
+      <c r="D29" s="18">
+        <v>36</v>
+      </c>
+      <c r="F29" s="15">
+        <f>B28+C29+D30</f>
+        <v>91</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="18">
+        <v>27</v>
+      </c>
+      <c r="C30" s="18">
+        <v>36</v>
+      </c>
+      <c r="D30" s="18">
+        <v>45</v>
+      </c>
+      <c r="F30" s="15">
+        <f>(B24^2+B25^2+B26^2+C24^2+C25^2+C26^2)</f>
+        <v>91</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="3">
+        <v>6</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+      <c r="E33" s="3">
+        <v>5</v>
+      </c>
+      <c r="F33" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="3">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3">
+        <v>4</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B37" s="19" cm="1">
+        <f t="array" ref="B37:C38">MMULT(B33:C34,E33:F34)</f>
+        <v>46</v>
+      </c>
+      <c r="C37" s="19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="19">
+        <v>27</v>
+      </c>
+      <c r="C38" s="19">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B41" s="19" cm="1">
+        <f t="array" ref="B41:C42">MINVERSE(_xlfn.ANCHORARRAY(B37))</f>
+        <v>5.5000000000000133</v>
+      </c>
+      <c r="C41" s="19">
+        <v>-9.3333333333333552</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B42" s="19">
+        <v>-4.5000000000000107</v>
+      </c>
+      <c r="C42" s="19">
+        <v>7.6666666666666847</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="F45" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" cm="1">
+        <f t="array" ref="B46:C47">MINVERSE(E33:F34)</f>
+        <v>5.0000000000000169</v>
+      </c>
+      <c r="C46" s="17">
+        <v>-6.0000000000000213</v>
+      </c>
+      <c r="F46" s="17" cm="1">
+        <f t="array" ref="F46:G47">MINVERSE(B33:C34)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="17">
+        <v>-0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="17">
+        <v>-4.0000000000000142</v>
+      </c>
+      <c r="C47" s="17">
+        <v>5.0000000000000178</v>
+      </c>
+      <c r="F47" s="17">
+        <v>-0.5</v>
+      </c>
+      <c r="G47" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="20" cm="1">
+        <f t="array" ref="B50:C51">MMULT(_xlfn.ANCHORARRAY(B46),_xlfn.ANCHORARRAY(F46))</f>
+        <v>5.5000000000000195</v>
+      </c>
+      <c r="C50" s="20">
+        <v>-9.3333333333333659</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" s="20">
+        <v>-4.500000000000016</v>
+      </c>
+      <c r="C51" s="20">
+        <v>7.6666666666666936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
matrix reviews and some text analysis
</commit_message>
<xml_diff>
--- a/7_MATHS/2_Matrix/1_Matrices.xlsx
+++ b/7_MATHS/2_Matrix/1_Matrices.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\7_MATHS\2_Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02E7D16-5FA0-490E-A7E8-CD22487116CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0687DB53-714A-44F4-892D-1F6F3D982F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Basic" sheetId="1" r:id="rId1"/>
+    <sheet name="Outer &amp; Inner" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Matrix A</t>
   </si>
@@ -245,12 +245,64 @@
       <t>-1</t>
     </r>
   </si>
+  <si>
+    <t>If matrix is invertible, then its inverse is UNIQUE as well e.g.</t>
+  </si>
+  <si>
+    <r>
+      <t>A + A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A - A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A . A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <t>. A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +358,13 @@
     </font>
     <font>
       <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,6 +487,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,7 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20:H23"/>
     </sheetView>
   </sheetViews>
@@ -1267,15 +1327,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EA0345-A843-4158-A3B6-4BAA3FA7F133}">
-  <dimension ref="B2:K51"/>
+  <dimension ref="B2:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="10"/>
     <col min="6" max="6" width="9.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="10"/>
   </cols>
@@ -1697,12 +1759,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" s="20" cm="1">
         <f t="array" ref="B50:C51">MMULT(_xlfn.ANCHORARRAY(B46),_xlfn.ANCHORARRAY(F46))</f>
         <v>5.5000000000000195</v>
@@ -1711,12 +1773,173 @@
         <v>-9.3333333333333659</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="20">
         <v>-4.500000000000016</v>
       </c>
       <c r="C51" s="20">
         <v>7.6666666666666936</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="E55" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B56" s="3">
+        <v>6</v>
+      </c>
+      <c r="C56" s="3">
+        <v>7</v>
+      </c>
+      <c r="E56" s="3" cm="1">
+        <f t="array" ref="E56:F57">MINVERSE(B56:C57)</f>
+        <v>-6.6666666666666693E-2</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0.46666666666666673</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B57" s="3">
+        <v>3</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F57" s="3">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="E60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="H60" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+      <c r="C61" s="3">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>2</v>
+      </c>
+      <c r="H61" s="10">
+        <f>B61+E61</f>
+        <v>2</v>
+      </c>
+      <c r="I61" s="10">
+        <f>C61+F61</f>
+        <v>4</v>
+      </c>
+      <c r="K61" s="10">
+        <f>B61-E61</f>
+        <v>0</v>
+      </c>
+      <c r="L61" s="10">
+        <f>C61-F61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B62" s="3">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3">
+        <v>4</v>
+      </c>
+      <c r="E62" s="3">
+        <v>2</v>
+      </c>
+      <c r="F62" s="3">
+        <v>4</v>
+      </c>
+      <c r="H62" s="10">
+        <f>B62+E62</f>
+        <v>4</v>
+      </c>
+      <c r="I62" s="10">
+        <f>C62+F62</f>
+        <v>8</v>
+      </c>
+      <c r="K62" s="10">
+        <f>B62-E62</f>
+        <v>0</v>
+      </c>
+      <c r="L62" s="10">
+        <f>C62-F62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" s="10" cm="1">
+        <f t="array" ref="B65:C66">MMULT(B61:C62,E61:F62)</f>
+        <v>5</v>
+      </c>
+      <c r="C65" s="10">
+        <v>10</v>
+      </c>
+      <c r="E65" s="10" cm="1">
+        <f t="array" ref="E65:F66">MMULT(E61:F62,B61:C62)</f>
+        <v>5</v>
+      </c>
+      <c r="F65" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="10">
+        <v>10</v>
+      </c>
+      <c r="C66" s="10">
+        <v>20</v>
+      </c>
+      <c r="E66" s="10">
+        <v>10</v>
+      </c>
+      <c r="F66" s="10">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review of openCV for image stitching
</commit_message>
<xml_diff>
--- a/7_MATHS/2_Matrix/1_Matrices.xlsx
+++ b/7_MATHS/2_Matrix/1_Matrices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\7_MATHS\2_Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0687DB53-714A-44F4-892D-1F6F3D982F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C4334B-71F0-4CF0-9E27-38D9EA49316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Matrix A</t>
   </si>
@@ -297,12 +297,55 @@
   <si>
     <t>. A</t>
   </si>
+  <si>
+    <t>Matrix Orthogonality</t>
+  </si>
+  <si>
+    <r>
+      <t>So for identity matrix A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>Orthogonal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +414,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -431,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -488,6 +546,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EA0345-A843-4158-A3B6-4BAA3FA7F133}">
-  <dimension ref="B2:L66"/>
+  <dimension ref="B2:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1942,6 +2001,184 @@
         <v>20</v>
       </c>
     </row>
+    <row r="68" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B68" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="E69" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" s="3">
+        <v>1</v>
+      </c>
+      <c r="C70" s="3">
+        <v>0</v>
+      </c>
+      <c r="E70" s="3" cm="1">
+        <f t="array" ref="E70:F71">MINVERSE(B70:C71)</f>
+        <v>1</v>
+      </c>
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="3">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="B73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="E73" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" s="3">
+        <v>1</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3" cm="1">
+        <f t="array" ref="E74:F75">TRANSPOSE(B74:C75)</f>
+        <v>1</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" s="3">
+        <v>0</v>
+      </c>
+      <c r="C75" s="3">
+        <v>1</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B79" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="E80" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B81" s="3">
+        <v>1</v>
+      </c>
+      <c r="C81" s="3">
+        <v>1</v>
+      </c>
+      <c r="E81" s="3" cm="1">
+        <f t="array" ref="E81:F82">MINVERSE(B81:C82)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F81" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H81" s="10">
+        <f>1/SQRT(2)</f>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B82" s="3">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F82" s="3">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="E84" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" s="1"/>
+      <c r="H84" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="3">
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="C85" s="3">
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E85" s="3" cm="1">
+        <f t="array" ref="E85:F86">MINVERSE(B85:C86)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.70710678118654779</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B86" s="3">
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="C86" s="3">
+        <v>-0.70710678118654702</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0.70710678118654779</v>
+      </c>
+      <c r="F86" s="3">
+        <v>-0.70710678118654779</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>